<commit_message>
Updated files from LSBC -- added new attribute
Signed-off-by: Stephen Curran <swcurran@gmail.com>
</commit_message>
<xml_diff>
--- a/OCABundles/schema/bcgov-digital-trust/LSBC/Membership/Prod/LSBC-OCA.xlsx
+++ b/OCABundles/schema/bcgov-digital-trust/LSBC/Membership/Prod/LSBC-OCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\_WebResources\Projects\digital credentials\aries-oca-bundles-main\OCABundles\schema\bcgov-digital-trust\lawyer-credential-PROD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03E252-3219-437A-B2B1-7C2591FCEFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167B8898-92B6-4A95-A3B7-D5ECF4CC6F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="1035" windowWidth="13800" windowHeight="11070" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start Here" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
   <si>
     <t>OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -2284,6 +2284,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2325,7 +2326,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -3050,28 +3050,28 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" ht="34.5" customHeight="1">
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="1:4" ht="39.75" customHeight="1">
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="80"/>
+      <c r="D5" s="81"/>
     </row>
     <row r="6" spans="1:4" ht="15">
       <c r="B6" s="5" t="s">
@@ -3091,10 +3091,10 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="81"/>
+      <c r="D8" s="82"/>
     </row>
     <row r="9" spans="1:4" ht="15">
       <c r="B9" s="5"/>
@@ -3110,31 +3110,31 @@
       <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
     </row>
     <row r="12" spans="1:4" ht="15">
       <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="10"/>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="10"/>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3190,11 +3190,11 @@
       <c r="D2" s="13"/>
     </row>
     <row r="3" spans="2:4" ht="93" customHeight="1">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
     </row>
     <row r="4" spans="2:4" ht="15">
       <c r="B4" s="3"/>
@@ -3213,7 +3213,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="79.5" customHeight="1">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -3224,7 +3224,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="60">
-      <c r="B7" s="86"/>
+      <c r="B7" s="87"/>
       <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
@@ -3233,7 +3233,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="60">
-      <c r="B8" s="86"/>
+      <c r="B8" s="87"/>
       <c r="C8" s="18" t="s">
         <v>21</v>
       </c>
@@ -3242,7 +3242,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="60">
-      <c r="B9" s="86"/>
+      <c r="B9" s="87"/>
       <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
@@ -3284,7 +3284,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="63.75" customHeight="1">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="88" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -3295,7 +3295,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="60">
-      <c r="B14" s="87"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="18" t="s">
         <v>37</v>
       </c>
@@ -3337,7 +3337,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="31.5" customHeight="1">
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="88" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -3348,7 +3348,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="30">
-      <c r="B19" s="87"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="18" t="s">
         <v>51</v>
       </c>
@@ -3390,7 +3390,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="88" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="21"/>
@@ -3399,7 +3399,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="30">
-      <c r="B24" s="87"/>
+      <c r="B24" s="88"/>
       <c r="C24" s="18" t="s">
         <v>64</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="45">
-      <c r="B25" s="87"/>
+      <c r="B25" s="88"/>
       <c r="C25" s="18" t="s">
         <v>66</v>
       </c>
@@ -3417,7 +3417,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="75">
-      <c r="B26" s="87"/>
+      <c r="B26" s="88"/>
       <c r="C26" s="18" t="s">
         <v>68</v>
       </c>
@@ -3426,7 +3426,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="30">
-      <c r="B27" s="87"/>
+      <c r="B27" s="88"/>
       <c r="C27" s="18" t="s">
         <v>70</v>
       </c>
@@ -3435,7 +3435,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="105">
-      <c r="B28" s="87"/>
+      <c r="B28" s="88"/>
       <c r="C28" s="18" t="s">
         <v>72</v>
       </c>
@@ -3444,7 +3444,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="60">
-      <c r="B29" s="87"/>
+      <c r="B29" s="88"/>
       <c r="C29" s="18" t="s">
         <v>74</v>
       </c>
@@ -3453,7 +3453,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="60">
-      <c r="B30" s="87"/>
+      <c r="B30" s="88"/>
       <c r="C30" s="18" t="s">
         <v>76</v>
       </c>
@@ -3485,18 +3485,18 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B34" s="82" t="s">
+      <c r="B34" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
     </row>
     <row r="35" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B35" s="83" t="s">
+      <c r="B35" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
     </row>
     <row r="36" spans="2:4" ht="15.75" customHeight="1">
       <c r="B36" s="25" t="s">
@@ -3560,16 +3560,16 @@
       <c r="D44" s="32"/>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B45" s="84" t="s">
+      <c r="B45" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="85"/>
     </row>
     <row r="46" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B46" s="76"/>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="77"/>
     </row>
     <row r="47" spans="2:4" ht="15.75" customHeight="1"/>
     <row r="48" spans="2:4" ht="15.75" customHeight="1"/>
@@ -4603,8 +4603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -4904,11 +4904,22 @@
       <c r="AA8" s="26"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="51"/>
+      <c r="A9" s="47" t="str">
+        <f>IF(AND(NOT(ISBLANK(A$4)),NOT($B9="")),A$4,"")</f>
+        <v/>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>101</v>
+      </c>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
@@ -36780,7 +36791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -37064,7 +37075,7 @@
       <c r="A10" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="73" t="s">
         <v>115</v>
       </c>
       <c r="C10" s="47" t="str">

</xml_diff>